<commit_message>
Upper respect and operators doubles
Los operadores dobles se comianel siguiente caracter, y cuando ingresaba
un id antes de unas cadena '' no respetaba el upper case
</commit_message>
<xml_diff>
--- a/judge.xlsx
+++ b/judge.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="190">
   <si>
     <t>&lt;proceso,1,1&gt;</t>
   </si>
@@ -570,13 +570,40 @@
   </si>
   <si>
     <t>&lt;token_cadena,├í,2,5&gt;</t>
+  </si>
+  <si>
+    <t>12.out</t>
+  </si>
+  <si>
+    <t>&lt;token_cor_izq,1,1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;id,asd,1,3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;token_mayor_igual,1,6&gt;</t>
+  </si>
+  <si>
+    <t>&lt;token_real,87678.9,1,8&gt;</t>
+  </si>
+  <si>
+    <t>&lt;token_cor_izq,2,1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;token_cor_der,2,2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;token_cor_der,2,4&gt;</t>
+  </si>
+  <si>
+    <t>:D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +639,14 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -633,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -656,6 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,12 +1006,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I200" sqref="I200"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1032,7 @@
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>111</v>
       </c>
@@ -1012,7 +1047,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>111</v>
       </c>
@@ -1027,7 +1062,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>111</v>
       </c>
@@ -1042,7 +1077,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>111</v>
       </c>
@@ -1057,7 +1092,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>111</v>
       </c>
@@ -1072,7 +1107,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>111</v>
       </c>
@@ -1087,7 +1122,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
@@ -1102,7 +1137,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
@@ -1113,7 +1148,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>112</v>
       </c>
@@ -1128,7 +1163,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>112</v>
       </c>
@@ -1143,7 +1178,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>112</v>
       </c>
@@ -1158,7 +1193,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>112</v>
       </c>
@@ -1173,7 +1208,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>112</v>
       </c>
@@ -1188,7 +1223,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>112</v>
       </c>
@@ -1203,7 +1238,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>112</v>
       </c>
@@ -1218,7 +1253,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>112</v>
       </c>
@@ -1233,7 +1268,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>112</v>
       </c>
@@ -1248,7 +1283,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>112</v>
       </c>
@@ -1263,7 +1298,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>112</v>
       </c>
@@ -1278,7 +1313,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>112</v>
       </c>
@@ -1293,7 +1328,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>112</v>
       </c>
@@ -1308,7 +1343,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>112</v>
       </c>
@@ -1319,7 +1354,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
@@ -1334,7 +1369,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>120</v>
       </c>
@@ -1349,7 +1384,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>120</v>
       </c>
@@ -1364,7 +1399,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>120</v>
       </c>
@@ -1379,7 +1414,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>120</v>
       </c>
@@ -1394,7 +1429,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>120</v>
       </c>
@@ -1409,7 +1444,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>120</v>
       </c>
@@ -1424,7 +1459,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
@@ -1439,7 +1474,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>120</v>
       </c>
@@ -1454,7 +1489,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>120</v>
       </c>
@@ -1469,7 +1504,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>120</v>
       </c>
@@ -1484,7 +1519,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>120</v>
       </c>
@@ -1499,7 +1534,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>120</v>
       </c>
@@ -1514,7 +1549,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>120</v>
       </c>
@@ -1524,7 +1559,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>27</v>
       </c>
@@ -1539,7 +1574,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>27</v>
       </c>
@@ -1554,7 +1589,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>27</v>
       </c>
@@ -1569,7 +1604,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>27</v>
       </c>
@@ -1584,7 +1619,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>27</v>
       </c>
@@ -1599,7 +1634,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>27</v>
       </c>
@@ -1614,7 +1649,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>27</v>
       </c>
@@ -1629,7 +1664,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>27</v>
       </c>
@@ -1644,7 +1679,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>27</v>
       </c>
@@ -1659,7 +1694,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>27</v>
       </c>
@@ -1674,7 +1709,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>27</v>
       </c>
@@ -1689,7 +1724,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>27</v>
       </c>
@@ -1704,7 +1739,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>27</v>
       </c>
@@ -1719,7 +1754,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>27</v>
       </c>
@@ -1734,7 +1769,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>27</v>
       </c>
@@ -1749,7 +1784,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>27</v>
       </c>
@@ -1764,7 +1799,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>27</v>
       </c>
@@ -1779,7 +1814,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>27</v>
       </c>
@@ -1794,7 +1829,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>27</v>
       </c>
@@ -1809,7 +1844,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>27</v>
       </c>
@@ -1824,7 +1859,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>27</v>
       </c>
@@ -1839,7 +1874,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>27</v>
       </c>
@@ -1854,7 +1889,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>27</v>
       </c>
@@ -1869,7 +1904,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>27</v>
       </c>
@@ -1884,7 +1919,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>27</v>
       </c>
@@ -1899,7 +1934,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>27</v>
       </c>
@@ -1914,7 +1949,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>27</v>
       </c>
@@ -1929,7 +1964,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>27</v>
       </c>
@@ -1939,7 +1974,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>38</v>
       </c>
@@ -1954,7 +1989,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>38</v>
       </c>
@@ -1969,7 +2004,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>38</v>
       </c>
@@ -1984,7 +2019,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>38</v>
       </c>
@@ -1999,7 +2034,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>38</v>
       </c>
@@ -2014,7 +2049,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>38</v>
       </c>
@@ -2029,7 +2064,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>38</v>
       </c>
@@ -2044,7 +2079,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>38</v>
       </c>
@@ -2059,7 +2094,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>38</v>
       </c>
@@ -2074,7 +2109,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>38</v>
       </c>
@@ -2089,7 +2124,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>38</v>
       </c>
@@ -2104,7 +2139,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>38</v>
       </c>
@@ -2119,7 +2154,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>38</v>
       </c>
@@ -2134,7 +2169,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>38</v>
       </c>
@@ -2149,7 +2184,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>38</v>
       </c>
@@ -2158,7 +2193,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>104</v>
       </c>
@@ -2173,7 +2208,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>104</v>
       </c>
@@ -2188,7 +2223,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>104</v>
       </c>
@@ -2203,7 +2238,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>104</v>
       </c>
@@ -2218,7 +2253,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>104</v>
       </c>
@@ -2233,7 +2268,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>104</v>
       </c>
@@ -2248,7 +2283,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>104</v>
       </c>
@@ -2263,7 +2298,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>104</v>
       </c>
@@ -2278,7 +2313,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>104</v>
       </c>
@@ -2293,7 +2328,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>104</v>
       </c>
@@ -2308,7 +2343,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>104</v>
       </c>
@@ -2323,7 +2358,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>104</v>
       </c>
@@ -2338,7 +2373,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>104</v>
       </c>
@@ -2353,7 +2388,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -2368,7 +2403,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>104</v>
       </c>
@@ -2383,7 +2418,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>104</v>
       </c>
@@ -2398,7 +2433,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>104</v>
       </c>
@@ -2413,7 +2448,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>104</v>
       </c>
@@ -2428,7 +2463,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>104</v>
       </c>
@@ -2443,7 +2478,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>104</v>
       </c>
@@ -2458,7 +2493,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>104</v>
       </c>
@@ -2473,7 +2508,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>104</v>
       </c>
@@ -2488,7 +2523,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>104</v>
       </c>
@@ -2503,7 +2538,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>104</v>
       </c>
@@ -2518,7 +2553,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>104</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>104</v>
       </c>
@@ -2548,7 +2583,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>104</v>
       </c>
@@ -2563,7 +2598,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>104</v>
       </c>
@@ -2578,7 +2613,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>104</v>
       </c>
@@ -2593,7 +2628,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>104</v>
       </c>
@@ -2608,7 +2643,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>104</v>
       </c>
@@ -2623,7 +2658,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>104</v>
       </c>
@@ -2638,7 +2673,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>104</v>
       </c>
@@ -2653,7 +2688,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>104</v>
       </c>
@@ -2668,7 +2703,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>104</v>
       </c>
@@ -2683,7 +2718,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>104</v>
       </c>
@@ -2698,7 +2733,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>104</v>
       </c>
@@ -2713,7 +2748,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>104</v>
       </c>
@@ -2728,7 +2763,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>104</v>
       </c>
@@ -2743,7 +2778,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>104</v>
       </c>
@@ -2758,7 +2793,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>104</v>
       </c>
@@ -2773,7 +2808,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>104</v>
       </c>
@@ -2788,7 +2823,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>104</v>
       </c>
@@ -2803,7 +2838,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>104</v>
       </c>
@@ -2818,7 +2853,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>104</v>
       </c>
@@ -2833,7 +2868,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>104</v>
       </c>
@@ -2848,7 +2883,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>104</v>
       </c>
@@ -2863,7 +2898,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>104</v>
       </c>
@@ -2878,7 +2913,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>104</v>
       </c>
@@ -2893,7 +2928,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>104</v>
       </c>
@@ -2908,7 +2943,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>104</v>
       </c>
@@ -2923,7 +2958,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>104</v>
       </c>
@@ -2938,7 +2973,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>104</v>
       </c>
@@ -2953,7 +2988,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>104</v>
       </c>
@@ -2968,7 +3003,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>104</v>
       </c>
@@ -2983,7 +3018,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>104</v>
       </c>
@@ -2998,7 +3033,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>104</v>
       </c>
@@ -3013,7 +3048,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>104</v>
       </c>
@@ -3028,7 +3063,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>104</v>
       </c>
@@ -3043,7 +3078,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>104</v>
       </c>
@@ -3058,7 +3093,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>104</v>
       </c>
@@ -3073,7 +3108,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>104</v>
       </c>
@@ -3088,7 +3123,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>104</v>
       </c>
@@ -3103,7 +3138,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>104</v>
       </c>
@@ -3118,7 +3153,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>104</v>
       </c>
@@ -3133,7 +3168,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>104</v>
       </c>
@@ -3148,7 +3183,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>104</v>
       </c>
@@ -3163,7 +3198,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>104</v>
       </c>
@@ -3172,7 +3207,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>133</v>
       </c>
@@ -3187,7 +3222,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>133</v>
       </c>
@@ -3202,7 +3237,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>133</v>
       </c>
@@ -3217,7 +3252,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>133</v>
       </c>
@@ -3232,7 +3267,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>133</v>
       </c>
@@ -3247,7 +3282,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>133</v>
       </c>
@@ -3262,7 +3297,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>133</v>
       </c>
@@ -3277,7 +3312,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>133</v>
       </c>
@@ -3292,7 +3327,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>133</v>
       </c>
@@ -3307,7 +3342,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>133</v>
       </c>
@@ -3322,7 +3357,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>133</v>
       </c>
@@ -3337,7 +3372,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>133</v>
       </c>
@@ -3352,7 +3387,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>133</v>
       </c>
@@ -3367,7 +3402,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>133</v>
       </c>
@@ -3382,7 +3417,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>133</v>
       </c>
@@ -3397,7 +3432,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>133</v>
       </c>
@@ -3412,7 +3447,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>133</v>
       </c>
@@ -3427,7 +3462,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>133</v>
       </c>
@@ -3442,7 +3477,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>133</v>
       </c>
@@ -3457,7 +3492,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>133</v>
       </c>
@@ -3466,7 +3501,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>151</v>
       </c>
@@ -3481,7 +3516,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>151</v>
       </c>
@@ -3496,7 +3531,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>151</v>
       </c>
@@ -3511,7 +3546,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>151</v>
       </c>
@@ -3526,7 +3561,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>151</v>
       </c>
@@ -3574,7 +3609,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>156</v>
       </c>
@@ -3589,7 +3624,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>156</v>
       </c>
@@ -3604,7 +3639,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>156</v>
       </c>
@@ -3619,7 +3654,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>156</v>
       </c>
@@ -3629,12 +3664,12 @@
       <c r="C180" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D180" t="str">
-        <f t="shared" si="6"/>
-        <v>:D</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D180" s="10" t="str">
+        <f t="shared" si="6"/>
+        <v>:D</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>156</v>
       </c>
@@ -3649,7 +3684,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>156</v>
       </c>
@@ -3664,7 +3699,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>156</v>
       </c>
@@ -3679,7 +3714,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>156</v>
       </c>
@@ -3694,7 +3729,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>156</v>
       </c>
@@ -3709,7 +3744,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>156</v>
       </c>
@@ -3724,7 +3759,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>156</v>
       </c>
@@ -3739,7 +3774,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>156</v>
       </c>
@@ -3754,7 +3789,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>156</v>
       </c>
@@ -3769,7 +3804,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>156</v>
       </c>
@@ -3784,7 +3819,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>156</v>
       </c>
@@ -3799,7 +3834,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>156</v>
       </c>
@@ -3814,7 +3849,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>156</v>
       </c>
@@ -3823,7 +3858,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>173</v>
       </c>
@@ -3838,7 +3873,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>173</v>
       </c>
@@ -3853,7 +3888,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>173</v>
       </c>
@@ -3868,7 +3903,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>173</v>
       </c>
@@ -3883,7 +3918,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>173</v>
       </c>
@@ -3892,14 +3927,106 @@
         <v>:D</v>
       </c>
     </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D199" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D200" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D201" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D202" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D203" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D204" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D205" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D198">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="9.out"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D198"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Upper respect and operators doubles"
This reverts commit 986d9c2ca888bc33e83ebe6cdd22f98f3c4e53b2.
</commit_message>
<xml_diff>
--- a/judge.xlsx
+++ b/judge.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="181">
   <si>
     <t>&lt;proceso,1,1&gt;</t>
   </si>
@@ -570,40 +570,13 @@
   </si>
   <si>
     <t>&lt;token_cadena,├í,2,5&gt;</t>
-  </si>
-  <si>
-    <t>12.out</t>
-  </si>
-  <si>
-    <t>&lt;token_cor_izq,1,1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;id,asd,1,3&gt;</t>
-  </si>
-  <si>
-    <t>&lt;token_mayor_igual,1,6&gt;</t>
-  </si>
-  <si>
-    <t>&lt;token_real,87678.9,1,8&gt;</t>
-  </si>
-  <si>
-    <t>&lt;token_cor_izq,2,1&gt;</t>
-  </si>
-  <si>
-    <t>&lt;token_cor_der,2,2&gt;</t>
-  </si>
-  <si>
-    <t>&lt;token_cor_der,2,4&gt;</t>
-  </si>
-  <si>
-    <t>:D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,14 +612,6 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -668,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -691,7 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,11 +970,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D205"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +997,7 @@
       </c>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>111</v>
       </c>
@@ -1047,7 +1012,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>111</v>
       </c>
@@ -1062,7 +1027,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>111</v>
       </c>
@@ -1077,7 +1042,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>111</v>
       </c>
@@ -1092,7 +1057,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>111</v>
       </c>
@@ -1107,7 +1072,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>111</v>
       </c>
@@ -1122,7 +1087,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
@@ -1137,7 +1102,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
@@ -1148,7 +1113,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>112</v>
       </c>
@@ -1163,7 +1128,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>112</v>
       </c>
@@ -1178,7 +1143,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>112</v>
       </c>
@@ -1193,7 +1158,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>112</v>
       </c>
@@ -1208,7 +1173,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>112</v>
       </c>
@@ -1223,7 +1188,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>112</v>
       </c>
@@ -1238,7 +1203,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>112</v>
       </c>
@@ -1253,7 +1218,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>112</v>
       </c>
@@ -1268,7 +1233,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>112</v>
       </c>
@@ -1283,7 +1248,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>112</v>
       </c>
@@ -1298,7 +1263,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>112</v>
       </c>
@@ -1313,7 +1278,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>112</v>
       </c>
@@ -1328,7 +1293,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>112</v>
       </c>
@@ -1343,7 +1308,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>112</v>
       </c>
@@ -1354,7 +1319,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
@@ -1369,7 +1334,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>120</v>
       </c>
@@ -1384,7 +1349,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>120</v>
       </c>
@@ -1399,7 +1364,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>120</v>
       </c>
@@ -1414,7 +1379,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>120</v>
       </c>
@@ -1429,7 +1394,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>120</v>
       </c>
@@ -1444,7 +1409,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>120</v>
       </c>
@@ -1459,7 +1424,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
@@ -1474,7 +1439,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>120</v>
       </c>
@@ -1489,7 +1454,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>120</v>
       </c>
@@ -1504,7 +1469,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>120</v>
       </c>
@@ -1519,7 +1484,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>120</v>
       </c>
@@ -1534,7 +1499,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>120</v>
       </c>
@@ -1549,7 +1514,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>120</v>
       </c>
@@ -1559,7 +1524,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>27</v>
       </c>
@@ -1574,7 +1539,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>27</v>
       </c>
@@ -1589,7 +1554,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>27</v>
       </c>
@@ -1604,7 +1569,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>27</v>
       </c>
@@ -1619,7 +1584,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>27</v>
       </c>
@@ -1634,7 +1599,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>27</v>
       </c>
@@ -1649,7 +1614,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1629,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>27</v>
       </c>
@@ -1679,7 +1644,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>27</v>
       </c>
@@ -1694,7 +1659,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>27</v>
       </c>
@@ -1709,7 +1674,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>27</v>
       </c>
@@ -1724,7 +1689,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>27</v>
       </c>
@@ -1739,7 +1704,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>27</v>
       </c>
@@ -1754,7 +1719,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>27</v>
       </c>
@@ -1769,7 +1734,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>27</v>
       </c>
@@ -1784,7 +1749,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>27</v>
       </c>
@@ -1799,7 +1764,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>27</v>
       </c>
@@ -1814,7 +1779,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>27</v>
       </c>
@@ -1829,7 +1794,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1809,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>27</v>
       </c>
@@ -1859,7 +1824,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>27</v>
       </c>
@@ -1874,7 +1839,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>27</v>
       </c>
@@ -1889,7 +1854,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>27</v>
       </c>
@@ -1904,7 +1869,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>27</v>
       </c>
@@ -1919,7 +1884,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +1899,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>27</v>
       </c>
@@ -1949,7 +1914,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>27</v>
       </c>
@@ -1964,7 +1929,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>27</v>
       </c>
@@ -1974,7 +1939,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>38</v>
       </c>
@@ -1989,7 +1954,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>38</v>
       </c>
@@ -2004,7 +1969,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>38</v>
       </c>
@@ -2019,7 +1984,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>38</v>
       </c>
@@ -2034,7 +1999,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>38</v>
       </c>
@@ -2049,7 +2014,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>38</v>
       </c>
@@ -2064,7 +2029,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>38</v>
       </c>
@@ -2079,7 +2044,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>38</v>
       </c>
@@ -2094,7 +2059,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>38</v>
       </c>
@@ -2109,7 +2074,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>38</v>
       </c>
@@ -2124,7 +2089,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>38</v>
       </c>
@@ -2139,7 +2104,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>38</v>
       </c>
@@ -2154,7 +2119,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>38</v>
       </c>
@@ -2169,7 +2134,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>38</v>
       </c>
@@ -2184,7 +2149,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>38</v>
       </c>
@@ -2193,7 +2158,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>104</v>
       </c>
@@ -2208,7 +2173,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>104</v>
       </c>
@@ -2223,7 +2188,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>104</v>
       </c>
@@ -2238,7 +2203,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>104</v>
       </c>
@@ -2253,7 +2218,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>104</v>
       </c>
@@ -2268,7 +2233,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>104</v>
       </c>
@@ -2283,7 +2248,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>104</v>
       </c>
@@ -2298,7 +2263,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>104</v>
       </c>
@@ -2313,7 +2278,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>104</v>
       </c>
@@ -2328,7 +2293,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>104</v>
       </c>
@@ -2343,7 +2308,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>104</v>
       </c>
@@ -2358,7 +2323,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>104</v>
       </c>
@@ -2373,7 +2338,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>104</v>
       </c>
@@ -2388,7 +2353,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -2403,7 +2368,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>104</v>
       </c>
@@ -2418,7 +2383,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>104</v>
       </c>
@@ -2433,7 +2398,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>104</v>
       </c>
@@ -2448,7 +2413,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>104</v>
       </c>
@@ -2463,7 +2428,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>104</v>
       </c>
@@ -2478,7 +2443,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>104</v>
       </c>
@@ -2493,7 +2458,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>104</v>
       </c>
@@ -2508,7 +2473,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>104</v>
       </c>
@@ -2523,7 +2488,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>104</v>
       </c>
@@ -2538,7 +2503,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>104</v>
       </c>
@@ -2553,7 +2518,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>104</v>
       </c>
@@ -2568,7 +2533,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>104</v>
       </c>
@@ -2583,7 +2548,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>104</v>
       </c>
@@ -2598,7 +2563,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>104</v>
       </c>
@@ -2613,7 +2578,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>104</v>
       </c>
@@ -2628,7 +2593,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>104</v>
       </c>
@@ -2643,7 +2608,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>104</v>
       </c>
@@ -2658,7 +2623,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>104</v>
       </c>
@@ -2673,7 +2638,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>104</v>
       </c>
@@ -2688,7 +2653,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>104</v>
       </c>
@@ -2703,7 +2668,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>104</v>
       </c>
@@ -2718,7 +2683,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>104</v>
       </c>
@@ -2733,7 +2698,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>104</v>
       </c>
@@ -2748,7 +2713,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>104</v>
       </c>
@@ -2763,7 +2728,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>104</v>
       </c>
@@ -2778,7 +2743,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>104</v>
       </c>
@@ -2793,7 +2758,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>104</v>
       </c>
@@ -2808,7 +2773,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>104</v>
       </c>
@@ -2823,7 +2788,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>104</v>
       </c>
@@ -2838,7 +2803,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>104</v>
       </c>
@@ -2853,7 +2818,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>104</v>
       </c>
@@ -2868,7 +2833,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>104</v>
       </c>
@@ -2883,7 +2848,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>104</v>
       </c>
@@ -2898,7 +2863,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>104</v>
       </c>
@@ -2913,7 +2878,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>104</v>
       </c>
@@ -2928,7 +2893,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>104</v>
       </c>
@@ -2943,7 +2908,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>104</v>
       </c>
@@ -2958,7 +2923,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>104</v>
       </c>
@@ -2973,7 +2938,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>104</v>
       </c>
@@ -2988,7 +2953,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>104</v>
       </c>
@@ -3003,7 +2968,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>104</v>
       </c>
@@ -3018,7 +2983,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>104</v>
       </c>
@@ -3033,7 +2998,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>104</v>
       </c>
@@ -3048,7 +3013,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>104</v>
       </c>
@@ -3063,7 +3028,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>104</v>
       </c>
@@ -3078,7 +3043,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>104</v>
       </c>
@@ -3093,7 +3058,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>104</v>
       </c>
@@ -3108,7 +3073,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>104</v>
       </c>
@@ -3123,7 +3088,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>104</v>
       </c>
@@ -3138,7 +3103,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>104</v>
       </c>
@@ -3153,7 +3118,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>104</v>
       </c>
@@ -3168,7 +3133,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>104</v>
       </c>
@@ -3183,7 +3148,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>104</v>
       </c>
@@ -3198,7 +3163,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>104</v>
       </c>
@@ -3207,7 +3172,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>133</v>
       </c>
@@ -3222,7 +3187,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>133</v>
       </c>
@@ -3237,7 +3202,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>133</v>
       </c>
@@ -3252,7 +3217,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>133</v>
       </c>
@@ -3267,7 +3232,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>133</v>
       </c>
@@ -3282,7 +3247,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>133</v>
       </c>
@@ -3297,7 +3262,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>133</v>
       </c>
@@ -3312,7 +3277,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>133</v>
       </c>
@@ -3327,7 +3292,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>133</v>
       </c>
@@ -3342,7 +3307,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>133</v>
       </c>
@@ -3357,7 +3322,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>133</v>
       </c>
@@ -3372,7 +3337,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>133</v>
       </c>
@@ -3387,7 +3352,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>133</v>
       </c>
@@ -3402,7 +3367,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>133</v>
       </c>
@@ -3417,7 +3382,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>133</v>
       </c>
@@ -3432,7 +3397,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>133</v>
       </c>
@@ -3447,7 +3412,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>133</v>
       </c>
@@ -3462,7 +3427,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>133</v>
       </c>
@@ -3477,7 +3442,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>133</v>
       </c>
@@ -3492,7 +3457,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>133</v>
       </c>
@@ -3501,7 +3466,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>151</v>
       </c>
@@ -3516,7 +3481,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>151</v>
       </c>
@@ -3531,7 +3496,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>151</v>
       </c>
@@ -3546,7 +3511,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>151</v>
       </c>
@@ -3561,7 +3526,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>151</v>
       </c>
@@ -3609,7 +3574,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>156</v>
       </c>
@@ -3624,7 +3589,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>156</v>
       </c>
@@ -3639,7 +3604,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>156</v>
       </c>
@@ -3654,7 +3619,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>156</v>
       </c>
@@ -3664,12 +3629,12 @@
       <c r="C180" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D180" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>:D</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D180" t="str">
+        <f t="shared" si="6"/>
+        <v>:D</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>156</v>
       </c>
@@ -3684,7 +3649,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>156</v>
       </c>
@@ -3699,7 +3664,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>156</v>
       </c>
@@ -3714,7 +3679,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>156</v>
       </c>
@@ -3729,7 +3694,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>156</v>
       </c>
@@ -3744,7 +3709,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>156</v>
       </c>
@@ -3759,7 +3724,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>156</v>
       </c>
@@ -3774,7 +3739,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>156</v>
       </c>
@@ -3789,7 +3754,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>156</v>
       </c>
@@ -3804,7 +3769,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>156</v>
       </c>
@@ -3819,7 +3784,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>156</v>
       </c>
@@ -3834,7 +3799,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>156</v>
       </c>
@@ -3849,7 +3814,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>156</v>
       </c>
@@ -3858,7 +3823,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>173</v>
       </c>
@@ -3873,7 +3838,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>173</v>
       </c>
@@ -3888,7 +3853,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>173</v>
       </c>
@@ -3903,7 +3868,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>173</v>
       </c>
@@ -3918,7 +3883,7 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>173</v>
       </c>
@@ -3927,106 +3892,14 @@
         <v>:D</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D199" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D200" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D201" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D202" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D203" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D204" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D205" t="s">
-        <v>189</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D198"/>
+  <autoFilter ref="A1:D198">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="9.out"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>